<commit_message>
adjustments to medication model, and allergy
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.allergyIntolerance.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.allergyIntolerance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="496">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-19T13:17:04-05:00</t>
+    <t>2023-07-21T16:23:00-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1468,6 +1468,9 @@
   </si>
   <si>
     <t>AllergyIntolerance.reaction.manifestation.coding.system</t>
+  </si>
+  <si>
+    <t>if code is 7 digits, then system is VUID, else use SNOMED-CT system</t>
   </si>
   <si>
     <t>AllergyIntolerance.reaction.manifestation.coding.version</t>
@@ -1944,7 +1947,7 @@
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="16.20703125" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="43.93359375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="46.46484375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="61.3671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9902,15 +9905,15 @@
         <v>305</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>40</v>
+        <v>461</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10021,10 +10024,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10130,15 +10133,15 @@
         <v>319</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10249,10 +10252,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10365,10 +10368,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10476,19 +10479,19 @@
         <v>344</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
@@ -10510,13 +10513,13 @@
         <v>60</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
@@ -10566,7 +10569,7 @@
         <v>40</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>38</v>
@@ -10581,7 +10584,7 @@
         <v>81</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -10595,10 +10598,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10624,10 +10627,10 @@
         <v>370</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -10678,7 +10681,7 @@
         <v>40</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>38</v>
@@ -10699,7 +10702,7 @@
         <v>40</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>40</v>
@@ -10707,10 +10710,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -10736,13 +10739,13 @@
         <v>124</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -10771,10 +10774,10 @@
         <v>180</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="Z78" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AA78" t="s" s="2">
         <v>40</v>
@@ -10792,7 +10795,7 @@
         <v>40</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>38</v>
@@ -10821,10 +10824,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -10850,13 +10853,13 @@
         <v>187</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
@@ -10885,10 +10888,10 @@
         <v>114</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>40</v>
@@ -10906,7 +10909,7 @@
         <v>40</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>38</v>
@@ -10921,7 +10924,7 @@
         <v>81</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
@@ -10935,10 +10938,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -10964,13 +10967,13 @@
         <v>400</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" t="s" s="2">
@@ -11020,7 +11023,7 @@
         <v>40</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>38</v>

</xml_diff>

<commit_message>
cleanup and improve mapping in Allergy and Immunization
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.allergyIntolerance.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.allergyIntolerance.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$91</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="550">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-03T12:49:33-05:00</t>
+    <t>2023-08-17T15:11:45-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -793,6 +793,9 @@
   </si>
   <si>
     <t>Observation ACT .inboundRelationship[typeCode=COMP].source[classCode=OBS, code="verificationStatus", moodCode=EVN].value</t>
+  </si>
+  <si>
+    <t>intoleranceCondition.informationSourceCategory: `OBSERVED` -&gt; `confirmed`;  `HISTORICAL` -&gt; `unconfirmed`</t>
   </si>
   <si>
     <t>AllergyIntolerance.type</t>
@@ -1231,6 +1234,173 @@
   </si>
   <si>
     <t>FiveWs.author</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.id</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension:visn</t>
+  </si>
+  <si>
+    <t>visn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {alternate-reference}
+</t>
+  </si>
+  <si>
+    <t>Alternative reference (target type is wrong)</t>
+  </si>
+  <si>
+    <t>Used when the target of the reference has a type that is not allowed by the definition of the element. In general, this should only arise when wrangling between versions using cross-version extensions.</t>
+  </si>
+  <si>
+    <t>Given that a reference SHALL have a display or reference, using this extension implies that there's a display present.</t>
+  </si>
+  <si>
+    <t>Organization(intoleranceCondition.facilityIdentifier)</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension:visn.id</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension:visn.extension</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension.extension</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension:visn.url</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension.url</t>
+  </si>
+  <si>
+    <t>identifies the meaning of the extension</t>
+  </si>
+  <si>
+    <t>Source of the definition for the extension code - a logical name or a URL.</t>
+  </si>
+  <si>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/alternate-reference</t>
+  </si>
+  <si>
+    <t>Extension.url</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension:visn.value[x]</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.extension.value[x]</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R5/extensibility.html) for a list).</t>
+  </si>
+  <si>
+    <t>Extension.value[x]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext-1
+</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.type</t>
+  </si>
+  <si>
+    <t>Type the reference refers to (e.g. "Patient")</t>
+  </si>
+  <si>
+    <t>The expected type of the target of the reference. If both Reference.type and Reference.reference are populated and Reference.reference is a FHIR URL, both SHALL be consistent.
+The type is the Canonical URL of Resource Definition that is the type this reference refers to. References are URLs that are relative to http://hl7.org/fhir/StructureDefinition/ e.g. "Patient" is a reference to http://hl7.org/fhir/StructureDefinition/Patient. Absolute URLs are only allowed for logical models (and can only be used in references in logical models, not resources).</t>
+  </si>
+  <si>
+    <t>This element is used to indicate the type of  the target of the reference. This may be used which ever of the other elements are populated (or not). In some cases, the type of the target may be determined by inspection of the reference (e.g. a RESTful URL) or by resolving the target of the reference; if both the type and a reference is provided, the reference SHALL resolve to a resource of the same type as that specified.</t>
+  </si>
+  <si>
+    <t>Aa resource (or, for logical models, the URI of the logical model).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+  </si>
+  <si>
+    <t>Reference.type</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.identifier</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the target resource. This is used when there is no way to reference the other resource directly, either because the entity it represents is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.
+Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.recorder.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
   </si>
   <si>
     <t>AllergyIntolerance.asserter</t>
@@ -1901,7 +2071,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN80"/>
+  <dimension ref="A1:AN91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1947,7 +2117,7 @@
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="16.20703125" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="43.93359375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="61.3671875" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="99.44140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5157,10 +5327,10 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>48</v>
@@ -5253,19 +5423,19 @@
         <v>40</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>40</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
@@ -5287,13 +5457,13 @@
         <v>124</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5322,10 +5492,10 @@
         <v>180</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>40</v>
@@ -5343,7 +5513,7 @@
         <v>40</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>38</v>
@@ -5358,13 +5528,13 @@
         <v>81</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>40</v>
@@ -5372,14 +5542,14 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -5401,13 +5571,13 @@
         <v>124</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5437,7 +5607,7 @@
       </c>
       <c r="Y31" s="2"/>
       <c r="Z31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>40</v>
@@ -5455,7 +5625,7 @@
         <v>40</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>38</v>
@@ -5470,28 +5640,28 @@
         <v>81</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5513,13 +5683,13 @@
         <v>124</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -5548,10 +5718,10 @@
         <v>180</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>40</v>
@@ -5569,7 +5739,7 @@
         <v>40</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>38</v>
@@ -5584,13 +5754,13 @@
         <v>81</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>40</v>
@@ -5598,14 +5768,14 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
@@ -5627,13 +5797,13 @@
         <v>187</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5663,7 +5833,7 @@
       </c>
       <c r="Y33" s="2"/>
       <c r="Z33" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>40</v>
@@ -5681,7 +5851,7 @@
         <v>40</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>38</v>
@@ -5696,13 +5866,13 @@
         <v>81</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>40</v>
@@ -5710,10 +5880,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5822,10 +5992,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5936,10 +6106,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5965,16 +6135,16 @@
         <v>102</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>40</v>
@@ -6023,7 +6193,7 @@
         <v>40</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>38</v>
@@ -6038,13 +6208,13 @@
         <v>81</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>40</v>
@@ -6052,10 +6222,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6164,10 +6334,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6278,10 +6448,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6307,16 +6477,16 @@
         <v>90</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>40</v>
@@ -6365,7 +6535,7 @@
         <v>40</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>38</v>
@@ -6380,13 +6550,13 @@
         <v>81</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>40</v>
@@ -6394,10 +6564,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6423,13 +6593,13 @@
         <v>60</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6479,7 +6649,7 @@
         <v>40</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>38</v>
@@ -6494,13 +6664,13 @@
         <v>81</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>40</v>
@@ -6508,10 +6678,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6537,14 +6707,14 @@
         <v>124</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>40</v>
@@ -6593,7 +6763,7 @@
         <v>40</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>38</v>
@@ -6608,13 +6778,13 @@
         <v>81</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>40</v>
@@ -6622,10 +6792,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6651,14 +6821,14 @@
         <v>60</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>40</v>
@@ -6707,7 +6877,7 @@
         <v>40</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>38</v>
@@ -6722,24 +6892,24 @@
         <v>81</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6762,19 +6932,19 @@
         <v>48</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>40</v>
@@ -6823,7 +6993,7 @@
         <v>40</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>38</v>
@@ -6838,13 +7008,13 @@
         <v>81</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>40</v>
@@ -6852,10 +7022,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6881,16 +7051,16 @@
         <v>60</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>40</v>
@@ -6939,7 +7109,7 @@
         <v>40</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>38</v>
@@ -6954,28 +7124,28 @@
         <v>81</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -6994,13 +7164,13 @@
         <v>48</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7051,7 +7221,7 @@
         <v>40</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>47</v>
@@ -7066,24 +7236,24 @@
         <v>81</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7106,13 +7276,13 @@
         <v>40</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7163,7 +7333,7 @@
         <v>40</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>38</v>
@@ -7178,10 +7348,10 @@
         <v>81</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>40</v>
@@ -7192,10 +7362,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7218,13 +7388,13 @@
         <v>40</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7263,7 +7433,7 @@
         <v>40</v>
       </c>
       <c r="AB47" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" t="s" s="2">
@@ -7273,7 +7443,7 @@
         <v>73</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>38</v>
@@ -7288,10 +7458,10 @@
         <v>81</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>40</v>
@@ -7302,13 +7472,13 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>40</v>
@@ -7330,13 +7500,13 @@
         <v>40</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7387,7 +7557,7 @@
         <v>40</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>38</v>
@@ -7402,24 +7572,24 @@
         <v>81</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7442,13 +7612,13 @@
         <v>40</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7499,7 +7669,7 @@
         <v>40</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>38</v>
@@ -7514,13 +7684,13 @@
         <v>81</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>40</v>
@@ -7528,14 +7698,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7554,13 +7724,13 @@
         <v>40</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7611,7 +7781,7 @@
         <v>40</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>38</v>
@@ -7626,10 +7796,10 @@
         <v>81</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>40</v>
@@ -7640,21 +7810,21 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>386</v>
+        <v>40</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>40</v>
@@ -7663,20 +7833,18 @@
         <v>40</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>387</v>
+        <v>60</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>388</v>
+        <v>61</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>390</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>40</v>
@@ -7725,7 +7893,7 @@
         <v>40</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>385</v>
+        <v>63</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>38</v>
@@ -7737,16 +7905,16 @@
         <v>40</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>391</v>
+        <v>64</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>392</v>
+        <v>40</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>393</v>
+        <v>40</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>40</v>
@@ -7754,21 +7922,21 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>40</v>
@@ -7780,16 +7948,16 @@
         <v>40</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>370</v>
+        <v>67</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>395</v>
+        <v>68</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>396</v>
+        <v>69</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>397</v>
+        <v>70</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7827,34 +7995,34 @@
         <v>40</v>
       </c>
       <c r="AB52" t="s" s="2">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="AC52" t="s" s="2">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="AD52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>394</v>
+        <v>74</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>398</v>
+        <v>64</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>40</v>
@@ -7868,12 +8036,14 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>387</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>389</v>
+      </c>
       <c r="D53" t="s" s="2">
         <v>40</v>
       </c>
@@ -7882,10 +8052,10 @@
         <v>38</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>40</v>
@@ -7894,16 +8064,16 @@
         <v>40</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7953,7 +8123,7 @@
         <v>40</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>399</v>
+        <v>74</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>38</v>
@@ -7965,10 +8135,10 @@
         <v>40</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>404</v>
+        <v>40</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>40</v>
@@ -7977,15 +8147,15 @@
         <v>40</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8008,7 +8178,7 @@
         <v>40</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="L54" t="s" s="2">
         <v>61</v>
@@ -8074,7 +8244,7 @@
         <v>47</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>40</v>
+        <v>397</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>40</v>
@@ -8094,21 +8264,21 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>40</v>
@@ -8123,14 +8293,12 @@
         <v>67</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>68</v>
+        <v>400</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>40</v>
@@ -8194,7 +8362,7 @@
         <v>75</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>40</v>
@@ -8208,10 +8376,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8219,10 +8387,10 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>40</v>
@@ -8231,19 +8399,19 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>409</v>
+        <v>90</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8251,7 +8419,7 @@
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" t="s" s="2">
-        <v>40</v>
+        <v>407</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>40</v>
@@ -8293,10 +8461,10 @@
         <v>40</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>47</v>
@@ -8305,16 +8473,16 @@
         <v>40</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>414</v>
+        <v>147</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>40</v>
@@ -8322,10 +8490,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8333,28 +8501,28 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>47</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>370</v>
+        <v>225</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8405,7 +8573,7 @@
         <v>40</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>38</v>
@@ -8414,30 +8582,30 @@
         <v>47</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>40</v>
+        <v>414</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>419</v>
+        <v>147</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>420</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8445,13 +8613,13 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>47</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I58" t="s" s="2">
         <v>40</v>
@@ -8460,15 +8628,17 @@
         <v>48</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>422</v>
+        <v>60</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="N58" s="2"/>
+        <v>417</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>418</v>
+      </c>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
         <v>40</v>
@@ -8517,39 +8687,39 @@
         <v>40</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>47</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>40</v>
+        <v>420</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>426</v>
+        <v>147</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>427</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8560,27 +8730,29 @@
         <v>38</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J59" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="I59" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J59" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="K59" t="s" s="2">
-        <v>429</v>
+        <v>90</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="N59" s="2"/>
+        <v>423</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>424</v>
+      </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>40</v>
@@ -8605,13 +8777,13 @@
         <v>40</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>40</v>
+        <v>425</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>40</v>
+        <v>426</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>40</v>
@@ -8629,13 +8801,13 @@
         <v>40</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>40</v>
@@ -8644,7 +8816,7 @@
         <v>81</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>432</v>
+        <v>147</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
@@ -8658,10 +8830,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8681,18 +8853,20 @@
         <v>40</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>61</v>
+        <v>429</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>430</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>431</v>
+      </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>40</v>
@@ -8741,7 +8915,7 @@
         <v>40</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>63</v>
+        <v>432</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>38</v>
@@ -8753,10 +8927,10 @@
         <v>40</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>64</v>
+        <v>433</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
@@ -8777,14 +8951,14 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>40</v>
@@ -8793,19 +8967,19 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>68</v>
+        <v>435</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>69</v>
+        <v>436</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>70</v>
+        <v>437</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
@@ -8855,22 +9029,22 @@
         <v>40</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>74</v>
+        <v>438</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>40</v>
@@ -8884,46 +9058,44 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
         <v>48</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>67</v>
+        <v>441</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>154</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>40</v>
       </c>
@@ -8977,22 +9149,22 @@
         <v>38</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>147</v>
+        <v>445</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>40</v>
+        <v>446</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>40</v>
+        <v>447</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>40</v>
@@ -9000,10 +9172,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9026,16 +9198,16 @@
         <v>40</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>187</v>
+        <v>371</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
@@ -9061,13 +9233,13 @@
         <v>40</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>444</v>
+        <v>40</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>445</v>
+        <v>40</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>40</v>
@@ -9085,7 +9257,7 @@
         <v>40</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>38</v>
@@ -9100,7 +9272,7 @@
         <v>81</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
@@ -9114,21 +9286,21 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>448</v>
+        <v>40</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>48</v>
@@ -9140,16 +9312,16 @@
         <v>40</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>187</v>
+        <v>454</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9175,11 +9347,13 @@
         <v>40</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="Y64" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Z64" t="s" s="2">
-        <v>452</v>
+        <v>40</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>40</v>
@@ -9197,10 +9371,10 @@
         <v>40</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>39</v>
@@ -9212,24 +9386,24 @@
         <v>81</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>255</v>
+        <v>458</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>453</v>
+        <v>40</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9338,10 +9512,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9452,10 +9626,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9466,7 +9640,7 @@
         <v>38</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>40</v>
@@ -9478,20 +9652,18 @@
         <v>48</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>102</v>
+        <v>463</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>289</v>
+        <v>464</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>290</v>
+        <v>465</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="O67" t="s" s="2">
-        <v>292</v>
-      </c>
+        <v>466</v>
+      </c>
+      <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
         <v>40</v>
       </c>
@@ -9539,13 +9711,13 @@
         <v>40</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>293</v>
+        <v>467</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH67" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AI67" t="s" s="2">
         <v>40</v>
@@ -9554,13 +9726,13 @@
         <v>81</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>294</v>
+        <v>468</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>295</v>
+        <v>147</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>40</v>
@@ -9568,10 +9740,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9585,22 +9757,22 @@
         <v>47</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>60</v>
+        <v>371</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>61</v>
+        <v>470</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>62</v>
+        <v>471</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -9651,7 +9823,7 @@
         <v>40</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>63</v>
+        <v>472</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>38</v>
@@ -9663,60 +9835,58 @@
         <v>40</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>64</v>
+        <v>473</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>40</v>
+        <v>474</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>67</v>
+        <v>476</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>68</v>
+        <v>477</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>478</v>
+      </c>
+      <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
         <v>40</v>
@@ -9753,51 +9923,51 @@
         <v>40</v>
       </c>
       <c r="AB69" t="s" s="2">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="AC69" t="s" s="2">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="AD69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>74</v>
+        <v>479</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>64</v>
+        <v>480</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>40</v>
+        <v>481</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>460</v>
+        <v>482</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>460</v>
+        <v>482</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -9808,32 +9978,28 @@
         <v>38</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>90</v>
+        <v>483</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>299</v>
+        <v>484</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="O70" t="s" s="2">
-        <v>302</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
         <v>40</v>
       </c>
@@ -9881,13 +10047,13 @@
         <v>40</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>303</v>
+        <v>482</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>40</v>
@@ -9896,24 +10062,24 @@
         <v>81</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>304</v>
+        <v>486</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>305</v>
+        <v>40</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>461</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>462</v>
+        <v>487</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>462</v>
+        <v>487</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -9933,20 +10099,18 @@
         <v>40</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>60</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>307</v>
+        <v>61</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>309</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N71" s="2"/>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
         <v>40</v>
@@ -9995,7 +10159,7 @@
         <v>40</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>310</v>
+        <v>63</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>38</v>
@@ -10007,16 +10171,16 @@
         <v>40</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>311</v>
+        <v>64</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>312</v>
+        <v>40</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>40</v>
@@ -10024,21 +10188,21 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>463</v>
+        <v>488</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>463</v>
+        <v>488</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>40</v>
@@ -10047,21 +10211,21 @@
         <v>40</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>314</v>
+        <v>68</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="N72" s="2"/>
-      <c r="O72" t="s" s="2">
-        <v>316</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
         <v>40</v>
       </c>
@@ -10109,72 +10273,74 @@
         <v>40</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>317</v>
+        <v>74</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH72" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>318</v>
+        <v>64</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>319</v>
+        <v>40</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>464</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>465</v>
+        <v>489</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>465</v>
+        <v>489</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
-        <v>40</v>
+        <v>490</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="J73" t="s" s="2">
         <v>48</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>321</v>
+        <v>491</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N73" s="2"/>
+        <v>492</v>
+      </c>
+      <c r="N73" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="O73" t="s" s="2">
-        <v>323</v>
+        <v>154</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>40</v>
@@ -10223,28 +10389,28 @@
         <v>40</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>324</v>
+        <v>493</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH73" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>325</v>
+        <v>147</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>326</v>
+        <v>40</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>40</v>
@@ -10252,10 +10418,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>466</v>
+        <v>494</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>466</v>
+        <v>494</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10266,7 +10432,7 @@
         <v>38</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>40</v>
@@ -10275,23 +10441,21 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>329</v>
+        <v>187</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>330</v>
+        <v>495</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>331</v>
+        <v>496</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>333</v>
-      </c>
+        <v>497</v>
+      </c>
+      <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
         <v>40</v>
       </c>
@@ -10315,13 +10479,13 @@
         <v>40</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>40</v>
+        <v>498</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>40</v>
+        <v>499</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>40</v>
@@ -10339,7 +10503,7 @@
         <v>40</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>334</v>
+        <v>494</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>38</v>
@@ -10354,13 +10518,13 @@
         <v>81</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>335</v>
+        <v>500</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>336</v>
+        <v>40</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>40</v>
@@ -10368,46 +10532,44 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>467</v>
+        <v>501</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>467</v>
+        <v>501</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
-        <v>40</v>
+        <v>502</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>47</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>338</v>
+        <v>503</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>339</v>
+        <v>504</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>341</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
         <v>40</v>
       </c>
@@ -10431,13 +10593,11 @@
         <v>40</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="Y75" s="2"/>
       <c r="Z75" t="s" s="2">
-        <v>40</v>
+        <v>506</v>
       </c>
       <c r="AA75" t="s" s="2">
         <v>40</v>
@@ -10455,13 +10615,13 @@
         <v>40</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>342</v>
+        <v>501</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AH75" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI75" t="s" s="2">
         <v>40</v>
@@ -10470,35 +10630,35 @@
         <v>81</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>343</v>
+        <v>256</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>344</v>
+        <v>507</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>468</v>
+        <v>508</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>469</v>
+        <v>509</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>469</v>
+        <v>509</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>470</v>
+        <v>40</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>40</v>
@@ -10513,14 +10673,12 @@
         <v>60</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>471</v>
+        <v>61</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>472</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>473</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
         <v>40</v>
@@ -10569,7 +10727,7 @@
         <v>40</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>469</v>
+        <v>63</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>38</v>
@@ -10581,10 +10739,10 @@
         <v>40</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>474</v>
+        <v>64</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -10598,21 +10756,21 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>475</v>
+        <v>510</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>475</v>
+        <v>510</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>40</v>
@@ -10624,15 +10782,17 @@
         <v>40</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>370</v>
+        <v>67</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>476</v>
+        <v>68</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="N77" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="N77" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
         <v>40</v>
@@ -10669,40 +10829,40 @@
         <v>40</v>
       </c>
       <c r="AB77" t="s" s="2">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="AC77" t="s" s="2">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="AD77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>475</v>
+        <v>74</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>366</v>
+        <v>64</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>478</v>
+        <v>40</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>40</v>
@@ -10710,10 +10870,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>479</v>
+        <v>511</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>479</v>
+        <v>511</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -10724,7 +10884,7 @@
         <v>38</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>40</v>
@@ -10733,21 +10893,23 @@
         <v>40</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>480</v>
+        <v>290</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>481</v>
+        <v>291</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>482</v>
-      </c>
-      <c r="O78" s="2"/>
+        <v>292</v>
+      </c>
+      <c r="O78" t="s" s="2">
+        <v>293</v>
+      </c>
       <c r="P78" t="s" s="2">
         <v>40</v>
       </c>
@@ -10771,13 +10933,13 @@
         <v>40</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>180</v>
+        <v>40</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>483</v>
+        <v>40</v>
       </c>
       <c r="Z78" t="s" s="2">
-        <v>484</v>
+        <v>40</v>
       </c>
       <c r="AA78" t="s" s="2">
         <v>40</v>
@@ -10795,13 +10957,13 @@
         <v>40</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>479</v>
+        <v>294</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AI78" t="s" s="2">
         <v>40</v>
@@ -10810,13 +10972,13 @@
         <v>81</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>40</v>
+        <v>296</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>40</v>
@@ -10824,10 +10986,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>485</v>
+        <v>512</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>485</v>
+        <v>512</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -10838,7 +11000,7 @@
         <v>38</v>
       </c>
       <c r="G79" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H79" t="s" s="2">
         <v>40</v>
@@ -10850,17 +11012,15 @@
         <v>40</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>187</v>
+        <v>60</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>486</v>
+        <v>61</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>488</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N79" s="2"/>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
         <v>40</v>
@@ -10885,13 +11045,13 @@
         <v>40</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>489</v>
+        <v>40</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>490</v>
+        <v>40</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>40</v>
@@ -10909,7 +11069,7 @@
         <v>40</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>485</v>
+        <v>63</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>38</v>
@@ -10921,10 +11081,10 @@
         <v>40</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>491</v>
+        <v>64</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
@@ -10938,21 +11098,21 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>492</v>
+        <v>513</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>492</v>
+        <v>513</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H80" t="s" s="2">
         <v>40</v>
@@ -10964,16 +11124,16 @@
         <v>40</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>400</v>
+        <v>67</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>493</v>
+        <v>68</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>494</v>
+        <v>69</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>495</v>
+        <v>70</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" t="s" s="2">
@@ -11011,19 +11171,19 @@
         <v>40</v>
       </c>
       <c r="AB80" t="s" s="2">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="AC80" t="s" s="2">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="AD80" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>492</v>
+        <v>74</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>38</v>
@@ -11035,23 +11195,1281 @@
         <v>40</v>
       </c>
       <c r="AJ80" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK80" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AL80" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM80" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AN80" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" hidden="true">
+      <c r="A81" t="s" s="2">
+        <v>514</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>514</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G81" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J81" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K81" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="L81" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="O81" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="P81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q81" s="2"/>
+      <c r="R81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH81" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ81" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="AK80" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AN80" t="s" s="2">
+      <c r="AK81" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AL81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM81" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AN81" t="s" s="2">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="82" hidden="true">
+      <c r="A82" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="B82" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G82" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J82" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K82" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="L82" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M82" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="N82" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="O82" s="2"/>
+      <c r="P82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q82" s="2"/>
+      <c r="R82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK82" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AL82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM82" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AN82" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" hidden="true">
+      <c r="A83" t="s" s="2">
+        <v>517</v>
+      </c>
+      <c r="B83" t="s" s="2">
+        <v>517</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G83" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J83" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K83" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L83" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="M83" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="N83" s="2"/>
+      <c r="O83" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="P83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q83" s="2"/>
+      <c r="R83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK83" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="AL83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM83" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AN83" t="s" s="2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="84" hidden="true">
+      <c r="A84" t="s" s="2">
+        <v>519</v>
+      </c>
+      <c r="B84" t="s" s="2">
+        <v>519</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G84" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J84" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K84" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="L84" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M84" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="N84" s="2"/>
+      <c r="O84" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="P84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q84" s="2"/>
+      <c r="R84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF84" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AG84" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH84" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ84" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK84" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AL84" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM84" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AN84" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" hidden="true">
+      <c r="A85" t="s" s="2">
+        <v>520</v>
+      </c>
+      <c r="B85" t="s" s="2">
+        <v>520</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G85" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J85" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K85" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="L85" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="O85" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="P85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q85" s="2"/>
+      <c r="R85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF85" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AG85" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH85" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK85" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM85" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AN85" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" hidden="true">
+      <c r="A86" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="B86" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E86" s="2"/>
+      <c r="F86" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G86" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J86" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="L86" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="M86" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="N86" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="O86" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="P86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q86" s="2"/>
+      <c r="R86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK86" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AL86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM86" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="AN86" t="s" s="2">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="87" hidden="true">
+      <c r="A87" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="B87" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" t="s" s="2">
+        <v>524</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="M87" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="N87" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="O87" s="2"/>
+      <c r="P87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q87" s="2"/>
+      <c r="R87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="AL87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AN87" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" hidden="true">
+      <c r="A88" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="B88" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="F88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="N88" s="2"/>
+      <c r="O88" s="2"/>
+      <c r="P88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q88" s="2"/>
+      <c r="R88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>532</v>
+      </c>
+      <c r="AN88" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" hidden="true">
+      <c r="A89" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="B89" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>534</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>535</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="O89" s="2"/>
+      <c r="P89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q89" s="2"/>
+      <c r="R89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM89" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AN89" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" hidden="true">
+      <c r="A90" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="B90" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="K90" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="N90" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="O90" s="2"/>
+      <c r="P90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q90" s="2"/>
+      <c r="R90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AN90" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" hidden="true">
+      <c r="A91" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="B91" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="O91" s="2"/>
+      <c r="P91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q91" s="2"/>
+      <c r="R91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AN91" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN80">
+  <autoFilter ref="A1:AN91">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11061,7 +12479,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI79">
+  <conditionalFormatting sqref="A2:AI90">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>